<commit_message>
Revised the error codes for [epp-07](#Test-Case-epp-07), and the data provider, so that elements that can be empty do not result in errors when empty values are accepted by the server.
</commit_message>
<xml_diff>
--- a/data/epp-07-data.xlsx
+++ b/data/epp-07-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gavin.brown/Code/icann/rst-test-specs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABF2569-DBFD-3140-8793-1FF9A9A856D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5E86D1-9DA1-1E40-A965-94EFEDC9DAFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{CD472396-4CFB-9A45-AA99-46F4E9CB8B91}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="TableNotes">Sheet1!$B$3</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="79">
   <si>
     <t>id</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>EPP_CONTACT_CREATE_SERVER_ACCEPTS_EMPTY_NAME</t>
-  </si>
-  <si>
-    <t>EPP_CONTACT_CREATE_SERVER_ACCEPTS_EMPTY_STREET</t>
   </si>
   <si>
     <t>EPP_CONTACT_CREATE_SERVER_ACCEPTS_EMPTY_CITY</t>
@@ -314,6 +311,21 @@
   </si>
   <si>
     <t>EPP_CONTACT_CREATE_SERVER_ACCEPTS_INVALID_VOICE</t>
+  </si>
+  <si>
+    <t>Voice extension</t>
+  </si>
+  <si>
+    <t>fax</t>
+  </si>
+  <si>
+    <t>faxExt</t>
+  </si>
+  <si>
+    <t>voiceExt</t>
+  </si>
+  <si>
+    <t>EPP_CONTACT_CREATE_SERVER_ACCEPTS_INVALID_FAX</t>
   </si>
 </sst>
 </file>
@@ -427,59 +439,119 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
@@ -717,8 +789,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}" name="DataProvider" displayName="DataProvider" ref="B7:Q39" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="B7:Q39" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}" name="DataProvider" displayName="DataProvider" ref="B7:T46" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="B7:T46" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -735,20 +807,26 @@
     <filterColumn colId="13" hiddenButton="1"/>
     <filterColumn colId="14" hiddenButton="1"/>
     <filterColumn colId="15" hiddenButton="1"/>
+    <filterColumn colId="16" hiddenButton="1"/>
+    <filterColumn colId="17" hiddenButton="1"/>
+    <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{4AE738EA-0F6E-7D4F-8E30-1F60F72D5773}" name="id" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{DF12F6BB-79CC-F24D-93DC-3FD6FC6C8768}" name="postalInfoType" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{1D25CBD0-E38C-F54D-ABC8-C6A8B886A51D}" name="name" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{4AA9FD28-BCDE-AC46-8EE4-06139D825534}" name="org" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{27140724-0327-9A4F-9F85-FF16C328500A}" name="street1" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{E6299384-0983-5544-9A93-511B5F60F481}" name="street2" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{80512F60-D82A-1840-94F4-555A17A2A1F5}" name="street3" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{C00E0E16-1AD2-D547-907C-6D34CCD3E954}" name="city" dataDxfId="8"/>
-    <tableColumn id="21" xr3:uid="{69BA67E8-AD8F-234A-B5B5-9F53C6B33B83}" name="sp" dataDxfId="7"/>
-    <tableColumn id="20" xr3:uid="{73BBAE87-BAA1-9844-96B2-063F6AE0F638}" name="pc" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{3F68DA74-847E-9544-B36C-356195B33309}" name="cc" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{B8837AE7-9F20-9E42-8FBA-70A3FF213BDD}" name="voice" dataDxfId="4"/>
+  <tableColumns count="19">
+    <tableColumn id="1" xr3:uid="{4AE738EA-0F6E-7D4F-8E30-1F60F72D5773}" name="id" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{DF12F6BB-79CC-F24D-93DC-3FD6FC6C8768}" name="postalInfoType" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{1D25CBD0-E38C-F54D-ABC8-C6A8B886A51D}" name="name" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{4AA9FD28-BCDE-AC46-8EE4-06139D825534}" name="org" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{27140724-0327-9A4F-9F85-FF16C328500A}" name="street1" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{E6299384-0983-5544-9A93-511B5F60F481}" name="street2" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{80512F60-D82A-1840-94F4-555A17A2A1F5}" name="street3" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{C00E0E16-1AD2-D547-907C-6D34CCD3E954}" name="city" dataDxfId="11"/>
+    <tableColumn id="21" xr3:uid="{69BA67E8-AD8F-234A-B5B5-9F53C6B33B83}" name="sp" dataDxfId="10"/>
+    <tableColumn id="20" xr3:uid="{73BBAE87-BAA1-9844-96B2-063F6AE0F638}" name="pc" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{3F68DA74-847E-9544-B36C-356195B33309}" name="cc" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{B8837AE7-9F20-9E42-8FBA-70A3FF213BDD}" name="voice" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{F626BC76-3A97-1549-970E-DFEB10BEC70E}" name="voiceExt" dataDxfId="6"/>
+    <tableColumn id="17" xr3:uid="{989647FD-6639-7B42-BB31-B4E64A67E948}" name="fax" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{4C9222C2-BEBD-F948-BD84-7BBC19C15D9F}" name="faxExt" dataDxfId="4"/>
     <tableColumn id="13" xr3:uid="{1CE4A02B-D8F9-3044-86DC-B2597CFBCAB3}" name="email" dataDxfId="3"/>
     <tableColumn id="14" xr3:uid="{75707043-79CF-5041-8096-1A1692CD8827}" name="authInfo" dataDxfId="2"/>
     <tableColumn id="15" xr3:uid="{00D82E93-146D-6544-AF62-0DE540BD8AA2}" name="passOrFail" dataDxfId="1"/>
@@ -1075,11 +1153,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D4FAA1-1060-DC4E-8B86-313DD9301EC2}">
-  <dimension ref="B2:Q39"/>
+  <dimension ref="B2:T46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28:Q34"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1093,16 +1169,19 @@
     <col min="11" max="11" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="76.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="2"/>
+    <col min="14" max="14" width="16.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="39.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="76.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="25" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:20" ht="25" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -1119,10 +1198,13 @@
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
-    </row>
-    <row r="3" spans="2:17" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+    </row>
+    <row r="3" spans="2:20" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -1139,8 +1221,11 @@
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -1157,10 +1242,13 @@
       <c r="O4" s="10"/>
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
-    </row>
-    <row r="5" spans="2:17" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+    </row>
+    <row r="5" spans="2:20" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -1177,8 +1265,11 @@
       <c r="O5" s="9"/>
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
@@ -1195,13 +1286,16 @@
       <c r="O6" s="11"/>
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>1</v>
@@ -1210,13 +1304,13 @@
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>3</v>
@@ -1234,541 +1328,643 @@
         <v>7</v>
       </c>
       <c r="N7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="P7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q7" s="2" t="s">
+      <c r="S7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="T7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:17" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:20" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="N8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="R8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="S8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="T8" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P9" s="5" t="s">
-        <v>35</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
       <c r="Q9" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="T9" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="I10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I10" s="2" t="s">
+      <c r="S11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="C14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="S14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="P13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C14" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T15" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D16" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="E17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="S17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="I18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="L19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="M20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="Q21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D23" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T23" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="F24" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="S24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T24" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="I25" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T25" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="L26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T26" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="L27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T27" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="L28" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="S28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T28" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="M29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="S29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T29" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="M30" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="S30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T30" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="M31" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="S31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T31" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="M32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="S32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T32" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="13:20" x14ac:dyDescent="0.2">
+      <c r="M33" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="S33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T33" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="13:20" x14ac:dyDescent="0.2">
+      <c r="M34" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="S34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T34" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="13:20" x14ac:dyDescent="0.2">
+      <c r="M35" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="S35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T35" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="13:20" x14ac:dyDescent="0.2">
+      <c r="O36" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="S36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T36" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="13:20" x14ac:dyDescent="0.2">
+      <c r="O37" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="S37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T37" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="13:20" x14ac:dyDescent="0.2">
+      <c r="O38" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="S38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T38" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="13:20" x14ac:dyDescent="0.2">
+      <c r="O39" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="S39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T39" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="13:20" x14ac:dyDescent="0.2">
+      <c r="O40" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="S40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T40" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="13:20" x14ac:dyDescent="0.2">
+      <c r="O41" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="S41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T41" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="13:20" x14ac:dyDescent="0.2">
+      <c r="O42" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T42" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="13:20" x14ac:dyDescent="0.2">
+      <c r="Q43" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T43" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="13:20" x14ac:dyDescent="0.2">
+      <c r="Q44" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S44" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T44" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="13:20" x14ac:dyDescent="0.2">
+      <c r="Q45" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="S45" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T45" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="13:20" x14ac:dyDescent="0.2">
+      <c r="Q46" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="P16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="E17" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="F18" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="I19" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q19" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="L20" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="M21" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q21" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="D22" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="P22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="D23" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q23" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="F24" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="P24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q24" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="I25" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q25" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="L26" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q26" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="L27" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q27" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="L28" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="P28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q28" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="M29" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="P29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q29" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="M30" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="P30" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q30" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="M31" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="P31" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q31" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="M32" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="P32" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q32" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="13:17" x14ac:dyDescent="0.2">
-      <c r="M33" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="P33" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q33" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="13:17" x14ac:dyDescent="0.2">
-      <c r="M34" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="P34" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q34" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="13:17" x14ac:dyDescent="0.2">
-      <c r="M35" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="N35" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P35" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q35" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="13:17" x14ac:dyDescent="0.2">
-      <c r="N36" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="P36" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q36" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="13:17" x14ac:dyDescent="0.2">
-      <c r="N37" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="P37" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q37" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="13:17" x14ac:dyDescent="0.2">
-      <c r="N38" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P38" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q38" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="13:17" x14ac:dyDescent="0.2">
-      <c r="N39" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="P39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q39" s="2" t="s">
-        <v>34</v>
+      <c r="S46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T46" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="B5:Q5"/>
-    <mergeCell ref="B4:Q4"/>
-    <mergeCell ref="B6:Q6"/>
+    <mergeCell ref="B2:T2"/>
+    <mergeCell ref="B3:T3"/>
+    <mergeCell ref="B5:T5"/>
+    <mergeCell ref="B4:T4"/>
+    <mergeCell ref="B6:T6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="M28:M32" numberStoredAsText="1"/>
-  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>

<commit_message>
update postalInfoType column to change "int" to "{AUTO}" (indicating a value determined by epp.supportedContactPostalInfoTypes)
</commit_message>
<xml_diff>
--- a/data/epp-07-data.xlsx
+++ b/data/epp-07-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gavin.brown/Code/rst-test-specs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DD608F-B990-9941-B6FE-1314CAEEB018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA66A72-8981-534D-BE82-91081D6A667B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{CD472396-4CFB-9A45-AA99-46F4E9CB8B91}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="79">
   <si>
     <t>id</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>errorCode</t>
-  </si>
-  <si>
-    <t>int</t>
   </si>
   <si>
     <t>EPP_CONTACT_CREATE_INFO_RESPONSE_NOT_1000</t>
@@ -1116,7 +1113,7 @@
   <dimension ref="B2:T45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:T5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1143,7 +1140,7 @@
   <sheetData>
     <row r="2" spans="2:20" ht="25" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -1166,7 +1163,7 @@
     </row>
     <row r="3" spans="2:20" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -1210,7 +1207,7 @@
     </row>
     <row r="5" spans="2:20" ht="128" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -1257,7 +1254,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>1</v>
@@ -1266,13 +1263,13 @@
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>3</v>
@@ -1290,13 +1287,13 @@
         <v>7</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P7" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>8</v>
@@ -1305,7 +1302,7 @@
         <v>9</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="T7" s="2" t="s">
         <v>10</v>
@@ -1313,605 +1310,605 @@
     </row>
     <row r="8" spans="2:20" s="4" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="K8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="N8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="M8" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q8" s="3" t="s">
+      <c r="R8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="R8" s="3" t="s">
+      <c r="S8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="S8" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="T8" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="H10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="T10" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="S10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T10" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T11" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="T11" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T12" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T13" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="T13" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C14" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C15" s="2" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.2">
       <c r="D16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="5:20" x14ac:dyDescent="0.2">
       <c r="E17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="S17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="5:20" x14ac:dyDescent="0.2">
       <c r="I18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="L18" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="S18" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="5:20" x14ac:dyDescent="0.2">
       <c r="L19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M19" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="M19" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="S19" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="5:20" x14ac:dyDescent="0.2">
       <c r="M20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q20" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Q20" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="S20" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="5:20" x14ac:dyDescent="0.2">
       <c r="E21" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="5:20" x14ac:dyDescent="0.2">
       <c r="E22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="5:20" x14ac:dyDescent="0.2">
       <c r="F23" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="5:20" x14ac:dyDescent="0.2">
       <c r="I24" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T24" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="S24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="T24" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="25" spans="5:20" x14ac:dyDescent="0.2">
       <c r="L25" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T25" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="5:20" x14ac:dyDescent="0.2">
       <c r="L26" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T26" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="5:20" x14ac:dyDescent="0.2">
       <c r="L27" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="S27" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T27" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="5:20" x14ac:dyDescent="0.2">
       <c r="M28" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="5:20" x14ac:dyDescent="0.2">
       <c r="M29" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T29" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="5:20" x14ac:dyDescent="0.2">
       <c r="M30" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T30" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="5:20" x14ac:dyDescent="0.2">
       <c r="M31" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T31" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="5:20" x14ac:dyDescent="0.2">
       <c r="M32" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T32" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="13:20" x14ac:dyDescent="0.2">
       <c r="M33" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T33" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="13:20" x14ac:dyDescent="0.2">
       <c r="M34" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T34" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="13:20" x14ac:dyDescent="0.2">
       <c r="O35" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S35" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T35" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="13:20" x14ac:dyDescent="0.2">
       <c r="O36" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S36" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T36" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="13:20" x14ac:dyDescent="0.2">
       <c r="O37" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T37" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="13:20" x14ac:dyDescent="0.2">
       <c r="O38" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S38" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T38" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="13:20" x14ac:dyDescent="0.2">
       <c r="O39" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T39" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="13:20" x14ac:dyDescent="0.2">
       <c r="O40" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S40" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T40" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="13:20" x14ac:dyDescent="0.2">
       <c r="O41" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S41" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T41" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="13:20" x14ac:dyDescent="0.2">
       <c r="Q42" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S42" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T42" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="13:20" x14ac:dyDescent="0.2">
       <c r="Q43" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S43" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T43" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="13:20" x14ac:dyDescent="0.2">
       <c r="Q44" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S44" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T44" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="13:20" x14ac:dyDescent="0.2">
       <c r="Q45" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T45" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>